<commit_message>
Change register state test
</commit_message>
<xml_diff>
--- a/Тест.xlsx
+++ b/Тест.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theex\Desktop\BSUIR\ТИ\Лабы\2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5384A7-004F-428C-9876-A571ED3E2571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC413ABE-90F0-4525-BF8C-CD8F8907807B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,12 +91,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -104,6 +98,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -122,19 +122,19 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -415,53 +415,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:Z31"/>
+  <dimension ref="B3:AV54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="3.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" style="2" customWidth="1"/>
     <col min="4" max="20" width="3.6640625" customWidth="1"/>
-    <col min="21" max="21" width="3.6640625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="3.6640625" style="2" customWidth="1"/>
     <col min="22" max="25" width="3.6640625" customWidth="1"/>
-    <col min="26" max="26" width="3.33203125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="3.33203125" style="2" customWidth="1"/>
+    <col min="27" max="49" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
       <c r="Z3" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>23</v>
       </c>
       <c r="D4">
@@ -515,7 +516,7 @@
       <c r="T4">
         <v>6</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="4">
         <v>5</v>
       </c>
       <c r="V4">
@@ -536,14 +537,14 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -555,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -564,25 +565,25 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <v>1</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
         <v>1</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -590,22 +591,22 @@
       <c r="T5">
         <v>1</v>
       </c>
-      <c r="U5" s="2">
-        <v>1</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="7">
+      <c r="U5" s="4">
+        <v>1</v>
+      </c>
+      <c r="V5" s="2">
+        <v>1</v>
+      </c>
+      <c r="W5" s="2">
+        <v>1</v>
+      </c>
+      <c r="X5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="3">
         <f>IF(_xlfn.XOR(C5,U5),1,0)</f>
         <v>0</v>
       </c>
@@ -614,11 +615,11 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -630,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -639,25 +640,25 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>1</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <v>1</v>
@@ -665,36 +666,35 @@
       <c r="S6">
         <v>1</v>
       </c>
-      <c r="T6" s="3">
-        <v>1</v>
-      </c>
-      <c r="U6" s="2">
-        <v>0</v>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6" s="4">
+        <v>1</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6">
-        <f>Z5</f>
-        <v>0</v>
-      </c>
-      <c r="Z6" s="7">
-        <f t="shared" ref="Z6:Z27" si="0">IF(_xlfn.XOR(C6,U6),1,0)</f>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <f t="shared" ref="Z6:Z50" si="0">IF(_xlfn.XOR(C6,U6),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="2">
-        <v>0</v>
+      <c r="C7" s="4">
+        <v>1</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -706,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -715,25 +715,25 @@
         <v>1</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <v>1</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <v>1</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7">
         <v>1</v>
@@ -744,26 +744,25 @@
       <c r="S7">
         <v>1</v>
       </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7" s="2">
-        <v>0</v>
+      <c r="T7" s="1">
+        <v>1</v>
+      </c>
+      <c r="U7" s="4">
+        <v>1</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7">
         <v>0</v>
       </c>
       <c r="Y7">
-        <f>Z6</f>
-        <v>1</v>
-      </c>
-      <c r="Z7" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -772,7 +771,7 @@
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8">
@@ -782,7 +781,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -791,25 +790,25 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
         <v>1</v>
@@ -821,44 +820,43 @@
         <v>1</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="U8" s="4">
+        <v>1</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8">
         <v>0</v>
       </c>
       <c r="X8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8">
-        <f t="shared" ref="X8:Y27" si="1">Z7</f>
-        <v>0</v>
-      </c>
-      <c r="Z8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -867,25 +865,25 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <v>1</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <v>1</v>
@@ -897,44 +895,43 @@
         <v>1</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="U9" s="4">
+        <v>1</v>
       </c>
       <c r="V9">
         <v>0</v>
       </c>
       <c r="W9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9">
         <v>0</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z9" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <f>IF(_xlfn.XOR(C9,U9),1,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>6</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -943,25 +940,25 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -973,34 +970,33 @@
         <v>1</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10" s="2">
+        <v>1</v>
+      </c>
+      <c r="U10" s="4">
         <v>0</v>
       </c>
       <c r="V10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10">
         <v>0</v>
       </c>
       <c r="X10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z10" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1009,8 +1005,8 @@
       <c r="B11">
         <v>7</v>
       </c>
-      <c r="C11" s="2">
-        <v>0</v>
+      <c r="C11" s="4">
+        <v>1</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1019,25 +1015,25 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
         <v>1</v>
@@ -1049,37 +1045,36 @@
         <v>1</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
         <v>0</v>
       </c>
-      <c r="U11" s="2">
-        <v>1</v>
+      <c r="U11" s="4">
+        <v>0</v>
       </c>
       <c r="V11">
         <v>0</v>
       </c>
       <c r="W11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z11" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1088,32 +1083,32 @@
       <c r="B12">
         <v>8</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="4">
         <v>1</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -1125,40 +1120,39 @@
         <v>1</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
         <v>0</v>
       </c>
       <c r="T12">
-        <v>1</v>
-      </c>
-      <c r="U12" s="2">
+        <v>0</v>
+      </c>
+      <c r="U12" s="4">
         <v>0</v>
       </c>
       <c r="V12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X12">
         <v>1</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z12" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1167,29 +1161,29 @@
       <c r="B13">
         <v>9</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1201,31 +1195,31 @@
         <v>1</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13">
         <v>0</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T13">
         <v>0</v>
       </c>
-      <c r="U13" s="2">
-        <v>1</v>
+      <c r="U13" s="4">
+        <v>0</v>
       </c>
       <c r="V13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13">
         <v>1</v>
@@ -1234,38 +1228,37 @@
         <v>1</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z13" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="C14" s="2">
-        <v>0</v>
+      <c r="C14" s="4">
+        <v>1</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1277,31 +1270,31 @@
         <v>1</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14">
         <v>0</v>
       </c>
       <c r="T14">
-        <v>1</v>
-      </c>
-      <c r="U14" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="U14" s="4">
+        <v>0</v>
       </c>
       <c r="V14">
         <v>1</v>
@@ -1313,10 +1306,9 @@
         <v>1</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z14" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1325,23 +1317,23 @@
       <c r="B15">
         <v>11</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="4">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1353,33 +1345,33 @@
         <v>1</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>1</v>
-      </c>
-      <c r="U15" s="2">
+        <v>0</v>
+      </c>
+      <c r="U15" s="4">
         <v>1</v>
       </c>
       <c r="V15">
@@ -1389,13 +1381,12 @@
         <v>1</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z15" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1404,20 +1395,20 @@
       <c r="B16">
         <v>12</v>
       </c>
-      <c r="C16" s="2">
-        <v>0</v>
+      <c r="C16" s="4">
+        <v>1</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1429,71 +1420,70 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16">
         <v>0</v>
       </c>
       <c r="R16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16">
         <v>1</v>
       </c>
-      <c r="U16" s="2">
+      <c r="U16" s="4">
         <v>1</v>
       </c>
       <c r="V16">
         <v>1</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X16">
         <v>1</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z16" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>13</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="4">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1505,31 +1495,31 @@
         <v>1</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17">
         <v>0</v>
       </c>
       <c r="O17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17">
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17">
         <v>1</v>
@@ -1537,11 +1527,11 @@
       <c r="T17">
         <v>1</v>
       </c>
-      <c r="U17" s="2">
+      <c r="U17" s="4">
         <v>1</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W17">
         <v>1</v>
@@ -1550,10 +1540,9 @@
         <v>0</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z17" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1562,14 +1551,14 @@
       <c r="B18">
         <v>14</v>
       </c>
-      <c r="C18" s="2">
-        <v>0</v>
+      <c r="C18" s="4">
+        <v>1</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1581,31 +1570,31 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
       <c r="P18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18">
         <v>1</v>
@@ -1616,8 +1605,8 @@
       <c r="T18">
         <v>1</v>
       </c>
-      <c r="U18" s="2">
-        <v>0</v>
+      <c r="U18" s="4">
+        <v>1</v>
       </c>
       <c r="V18">
         <v>1</v>
@@ -1626,13 +1615,12 @@
         <v>0</v>
       </c>
       <c r="X18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z18" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1641,11 +1629,11 @@
       <c r="B19">
         <v>15</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="4">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1657,31 +1645,31 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19">
         <v>0</v>
       </c>
       <c r="O19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q19">
         <v>1</v>
@@ -1693,25 +1681,24 @@
         <v>1</v>
       </c>
       <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19" s="2">
+        <v>1</v>
+      </c>
+      <c r="U19" s="4">
         <v>1</v>
       </c>
       <c r="V19">
         <v>0</v>
       </c>
       <c r="W19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X19">
         <v>0</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z19" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1720,8 +1707,8 @@
       <c r="B20">
         <v>16</v>
       </c>
-      <c r="C20" s="2">
-        <v>0</v>
+      <c r="C20" s="4">
+        <v>1</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1733,31 +1720,31 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P20">
         <v>1</v>
@@ -1769,16 +1756,16 @@
         <v>1</v>
       </c>
       <c r="S20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20">
         <v>1</v>
       </c>
-      <c r="U20" s="2">
+      <c r="U20" s="4">
         <v>0</v>
       </c>
       <c r="V20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W20">
         <v>0</v>
@@ -1787,19 +1774,18 @@
         <v>0</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z20" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>17</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="4">
         <v>1</v>
       </c>
       <c r="D21">
@@ -1809,31 +1795,31 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21">
         <v>1</v>
@@ -1845,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21">
         <v>1</v>
@@ -1853,8 +1839,8 @@
       <c r="T21">
         <v>0</v>
       </c>
-      <c r="U21" s="2">
-        <v>1</v>
+      <c r="U21" s="4">
+        <v>0</v>
       </c>
       <c r="V21">
         <v>0</v>
@@ -1866,50 +1852,49 @@
         <v>0</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z21" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>18</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="4">
         <v>1</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -1921,7 +1906,7 @@
         <v>1</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22">
         <v>1</v>
@@ -1930,9 +1915,9 @@
         <v>0</v>
       </c>
       <c r="T22">
-        <v>1</v>
-      </c>
-      <c r="U22" s="2">
+        <v>0</v>
+      </c>
+      <c r="U22" s="4">
         <v>0</v>
       </c>
       <c r="V22">
@@ -1942,13 +1927,12 @@
         <v>0</v>
       </c>
       <c r="X22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z22" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1957,35 +1941,35 @@
       <c r="B23">
         <v>19</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="4">
         <v>1</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -1997,7 +1981,7 @@
         <v>1</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23">
         <v>1</v>
@@ -2006,28 +1990,27 @@
         <v>0</v>
       </c>
       <c r="S23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T23">
         <v>0</v>
       </c>
-      <c r="U23" s="2">
+      <c r="U23" s="4">
         <v>0</v>
       </c>
       <c r="V23">
         <v>0</v>
       </c>
       <c r="W23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z23" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2036,32 +2019,32 @@
       <c r="B24">
         <v>20</v>
       </c>
-      <c r="C24" s="2">
-        <v>0</v>
+      <c r="C24" s="4">
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -2073,7 +2056,7 @@
         <v>1</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24">
         <v>1</v>
@@ -2082,7 +2065,7 @@
         <v>0</v>
       </c>
       <c r="R24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S24">
         <v>0</v>
@@ -2090,54 +2073,53 @@
       <c r="T24">
         <v>0</v>
       </c>
-      <c r="U24" s="2">
+      <c r="U24" s="4">
         <v>0</v>
       </c>
       <c r="V24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X24">
         <v>1</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z24" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>21</v>
       </c>
-      <c r="C25" s="2">
-        <v>0</v>
+      <c r="C25" s="4">
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -2149,7 +2131,7 @@
         <v>1</v>
       </c>
       <c r="N25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25">
         <v>1</v>
@@ -2158,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R25">
         <v>0</v>
@@ -2169,11 +2151,11 @@
       <c r="T25">
         <v>0</v>
       </c>
-      <c r="U25" s="2">
-        <v>0</v>
+      <c r="U25" s="4">
+        <v>1</v>
       </c>
       <c r="V25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W25">
         <v>1</v>
@@ -2182,10 +2164,9 @@
         <v>1</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z25" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2194,26 +2175,26 @@
       <c r="B26">
         <v>22</v>
       </c>
-      <c r="C26" s="2">
-        <v>0</v>
+      <c r="C26" s="4">
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -2225,7 +2206,7 @@
         <v>1</v>
       </c>
       <c r="M26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -2234,7 +2215,7 @@
         <v>0</v>
       </c>
       <c r="P26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -2246,10 +2227,10 @@
         <v>0</v>
       </c>
       <c r="T26">
-        <v>0</v>
-      </c>
-      <c r="U26" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="U26" s="4">
+        <v>1</v>
       </c>
       <c r="V26">
         <v>1</v>
@@ -2258,13 +2239,12 @@
         <v>1</v>
       </c>
       <c r="X26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z26" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2273,23 +2253,23 @@
       <c r="B27">
         <v>23</v>
       </c>
-      <c r="C27" s="2">
-        <v>0</v>
+      <c r="C27" s="4">
+        <v>1</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -2301,7 +2281,7 @@
         <v>1</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -2310,7 +2290,7 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P27">
         <v>0</v>
@@ -2322,151 +2302,2013 @@
         <v>0</v>
       </c>
       <c r="S27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T27">
-        <v>0</v>
-      </c>
-      <c r="U27" s="2">
+        <v>1</v>
+      </c>
+      <c r="U27" s="4">
         <v>1</v>
       </c>
       <c r="V27">
         <v>1</v>
       </c>
       <c r="W27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X27">
         <v>0</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z27" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="3">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>24</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="U28" s="4">
+        <v>1</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="3">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
+      <c r="B29">
+        <v>25</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="U29" s="4">
+        <v>1</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="C30" s="5" t="s">
+      <c r="B30">
+        <v>26</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>1</v>
+      </c>
+      <c r="U30" s="4">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>1</v>
+      </c>
+      <c r="Y30">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>27</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31" s="4">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>1</v>
+      </c>
+      <c r="X31">
+        <v>1</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>28</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32" s="4">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>29</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33" s="4">
+        <v>1</v>
+      </c>
+      <c r="V33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>1</v>
+      </c>
+      <c r="U34" s="4">
+        <v>1</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>31</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+      <c r="T35">
+        <v>1</v>
+      </c>
+      <c r="U35" s="4">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>32</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36" s="4">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>33</v>
+      </c>
+      <c r="C37" s="4">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>1</v>
+      </c>
+      <c r="R37">
+        <v>1</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37" s="4">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <v>1</v>
+      </c>
+      <c r="Y37">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>34</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38" s="4">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>1</v>
+      </c>
+      <c r="X38">
+        <v>1</v>
+      </c>
+      <c r="Y38">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>35</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39" s="4">
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <v>1</v>
+      </c>
+      <c r="W39">
+        <v>1</v>
+      </c>
+      <c r="X39">
+        <v>1</v>
+      </c>
+      <c r="Y39">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>36</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40" s="4">
+        <v>1</v>
+      </c>
+      <c r="V40">
+        <v>1</v>
+      </c>
+      <c r="W40">
+        <v>1</v>
+      </c>
+      <c r="X40">
+        <v>0</v>
+      </c>
+      <c r="Y40">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>37</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="U41" s="4">
+        <v>1</v>
+      </c>
+      <c r="V41">
+        <v>1</v>
+      </c>
+      <c r="W41">
+        <v>0</v>
+      </c>
+      <c r="X41">
+        <v>0</v>
+      </c>
+      <c r="Y41">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>38</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
+      </c>
+      <c r="T42">
+        <v>1</v>
+      </c>
+      <c r="U42" s="4">
+        <v>1</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42">
+        <v>0</v>
+      </c>
+      <c r="X42">
+        <v>1</v>
+      </c>
+      <c r="Y42">
+        <v>1</v>
+      </c>
+      <c r="Z42" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>39</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>1</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
+      </c>
+      <c r="T43">
+        <v>1</v>
+      </c>
+      <c r="U43" s="4">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <v>0</v>
+      </c>
+      <c r="W43">
+        <v>1</v>
+      </c>
+      <c r="X43">
+        <v>1</v>
+      </c>
+      <c r="Y43">
+        <v>1</v>
+      </c>
+      <c r="Z43" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>40</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+      <c r="S44">
+        <v>1</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44" s="4">
+        <v>0</v>
+      </c>
+      <c r="V44">
+        <v>1</v>
+      </c>
+      <c r="W44">
+        <v>1</v>
+      </c>
+      <c r="X44">
+        <v>1</v>
+      </c>
+      <c r="Y44">
+        <v>1</v>
+      </c>
+      <c r="Z44" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>41</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="Q45">
+        <v>1</v>
+      </c>
+      <c r="R45">
+        <v>1</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+      <c r="U45" s="4">
+        <v>1</v>
+      </c>
+      <c r="V45">
+        <v>1</v>
+      </c>
+      <c r="W45">
+        <v>1</v>
+      </c>
+      <c r="X45">
+        <v>1</v>
+      </c>
+      <c r="Y45">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>42</v>
+      </c>
+      <c r="C46" s="4">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>1</v>
+      </c>
+      <c r="Q46">
+        <v>1</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>1</v>
+      </c>
+      <c r="U46" s="4">
+        <v>1</v>
+      </c>
+      <c r="V46">
+        <v>1</v>
+      </c>
+      <c r="W46">
+        <v>1</v>
+      </c>
+      <c r="X46">
+        <v>1</v>
+      </c>
+      <c r="Y46">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>43</v>
+      </c>
+      <c r="C47" s="4">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>1</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>1</v>
+      </c>
+      <c r="T47">
+        <v>1</v>
+      </c>
+      <c r="U47" s="4">
+        <v>1</v>
+      </c>
+      <c r="V47">
+        <v>1</v>
+      </c>
+      <c r="W47">
+        <v>1</v>
+      </c>
+      <c r="X47">
+        <v>0</v>
+      </c>
+      <c r="Y47">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>44</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>1</v>
+      </c>
+      <c r="S48">
+        <v>1</v>
+      </c>
+      <c r="T48">
+        <v>1</v>
+      </c>
+      <c r="U48" s="4">
+        <v>1</v>
+      </c>
+      <c r="V48">
+        <v>1</v>
+      </c>
+      <c r="W48">
+        <v>0</v>
+      </c>
+      <c r="X48">
+        <v>0</v>
+      </c>
+      <c r="Y48">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>45</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <v>1</v>
+      </c>
+      <c r="R49">
+        <v>1</v>
+      </c>
+      <c r="S49">
+        <v>1</v>
+      </c>
+      <c r="T49">
+        <v>1</v>
+      </c>
+      <c r="U49" s="4">
+        <v>1</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>0</v>
+      </c>
+      <c r="X49">
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <v>1</v>
+      </c>
+      <c r="Z49" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>46</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>1</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+      <c r="S50">
+        <v>1</v>
+      </c>
+      <c r="T50">
+        <v>1</v>
+      </c>
+      <c r="U50" s="4">
+        <v>0</v>
+      </c>
+      <c r="V50">
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <v>0</v>
+      </c>
+      <c r="X50">
+        <v>1</v>
+      </c>
+      <c r="Y50">
+        <v>1</v>
+      </c>
+      <c r="Z50" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="C53" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
-      <c r="U30" s="5"/>
-      <c r="V30" s="5"/>
-      <c r="W30" s="5"/>
-      <c r="X30" s="5"/>
-      <c r="Y30" s="5"/>
-    </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="C31" s="4" cm="1">
-        <f t="array" ref="C31:Y31">TRANSPOSE(C5:C27)</f>
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <v>1</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <v>1</v>
-      </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <v>1</v>
-      </c>
-      <c r="R31">
-        <v>0</v>
-      </c>
-      <c r="S31">
-        <v>1</v>
-      </c>
-      <c r="T31">
-        <v>1</v>
-      </c>
-      <c r="U31" s="4">
-        <v>1</v>
-      </c>
-      <c r="V31">
-        <v>0</v>
-      </c>
-      <c r="W31">
-        <v>0</v>
-      </c>
-      <c r="X31">
-        <v>0</v>
-      </c>
-      <c r="Y31">
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+      <c r="S53" s="7"/>
+      <c r="T53" s="7"/>
+      <c r="U53" s="7"/>
+      <c r="V53" s="7"/>
+      <c r="W53" s="7"/>
+      <c r="X53" s="7"/>
+      <c r="Y53" s="7"/>
+      <c r="Z53" s="7"/>
+      <c r="AA53" s="7"/>
+      <c r="AB53" s="7"/>
+      <c r="AC53" s="7"/>
+      <c r="AD53" s="7"/>
+      <c r="AE53" s="7"/>
+      <c r="AF53" s="7"/>
+      <c r="AG53" s="7"/>
+      <c r="AH53" s="7"/>
+      <c r="AI53" s="7"/>
+      <c r="AJ53" s="7"/>
+      <c r="AK53" s="7"/>
+      <c r="AL53" s="7"/>
+      <c r="AM53" s="7"/>
+      <c r="AN53" s="7"/>
+      <c r="AO53" s="7"/>
+      <c r="AP53" s="7"/>
+      <c r="AQ53" s="7"/>
+      <c r="AR53" s="7"/>
+      <c r="AS53" s="7"/>
+      <c r="AT53" s="7"/>
+      <c r="AU53" s="7"/>
+      <c r="AV53" s="7"/>
+    </row>
+    <row r="54" spans="2:48" x14ac:dyDescent="0.3">
+      <c r="C54" s="2" cm="1">
+        <f t="array" ref="C54:AV54">TRANSPOSE(C5:C50)</f>
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>1</v>
+      </c>
+      <c r="P54">
+        <v>1</v>
+      </c>
+      <c r="Q54">
+        <v>1</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
+      <c r="S54">
+        <v>1</v>
+      </c>
+      <c r="T54">
+        <v>1</v>
+      </c>
+      <c r="U54" s="2">
+        <v>1</v>
+      </c>
+      <c r="V54">
+        <v>1</v>
+      </c>
+      <c r="W54">
+        <v>1</v>
+      </c>
+      <c r="X54">
+        <v>1</v>
+      </c>
+      <c r="Y54">
+        <v>1</v>
+      </c>
+      <c r="Z54" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA54">
+        <v>0</v>
+      </c>
+      <c r="AB54">
+        <v>0</v>
+      </c>
+      <c r="AC54">
+        <v>0</v>
+      </c>
+      <c r="AD54">
+        <v>0</v>
+      </c>
+      <c r="AE54">
+        <v>1</v>
+      </c>
+      <c r="AF54">
+        <v>1</v>
+      </c>
+      <c r="AG54">
+        <v>1</v>
+      </c>
+      <c r="AH54">
+        <v>1</v>
+      </c>
+      <c r="AI54">
+        <v>1</v>
+      </c>
+      <c r="AJ54">
+        <v>0</v>
+      </c>
+      <c r="AK54">
+        <v>0</v>
+      </c>
+      <c r="AL54">
+        <v>0</v>
+      </c>
+      <c r="AM54">
+        <v>0</v>
+      </c>
+      <c r="AN54">
+        <v>0</v>
+      </c>
+      <c r="AO54">
+        <v>1</v>
+      </c>
+      <c r="AP54">
+        <v>1</v>
+      </c>
+      <c r="AQ54">
+        <v>1</v>
+      </c>
+      <c r="AR54">
+        <v>1</v>
+      </c>
+      <c r="AS54">
+        <v>1</v>
+      </c>
+      <c r="AT54">
+        <v>0</v>
+      </c>
+      <c r="AU54">
+        <v>0</v>
+      </c>
+      <c r="AV54">
         <v>0</v>
       </c>
     </row>
@@ -2474,7 +4316,7 @@
   <mergeCells count="3">
     <mergeCell ref="C3:Y3"/>
     <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="C30:Y30"/>
+    <mergeCell ref="C53:AV53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>